<commit_message>
The neos_flag parameter has been introduced as input variable in the optimization problem
</commit_message>
<xml_diff>
--- a/Inverse_Optimization_Related_Problem/temporary_results_inverse_optimization_related_problem/Output.xlsx
+++ b/Inverse_Optimization_Related_Problem/temporary_results_inverse_optimization_related_problem/Output.xlsx
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>29.32557511329651</v>
+        <v>1.07711935043335</v>
       </c>
     </row>
   </sheetData>
@@ -1685,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-6.228840434616256e-11</v>
+        <v>-0.01848287542273457</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1693,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4.664744579222947e-13</v>
+        <v>0.6217241268499804</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1701,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4.664842482827188e-13</v>
+        <v>-0.01862054293010882</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1709,7 +1709,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.664751266626648e-13</v>
+        <v>-0.01805540567109086</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1717,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4.664778625257313e-13</v>
+        <v>-0.01822347440889039</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1725,7 +1725,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4.664735085005177e-13</v>
+        <v>0.6894393787108369</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1733,7 +1733,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4.664762151897511e-13</v>
+        <v>-0.01812047942907844</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1741,7 +1741,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4.664809439505297e-13</v>
+        <v>-0.01841062349237289</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1749,7 +1749,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4.664763241927171e-13</v>
+        <v>-0.01812674857001915</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1757,7 +1757,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4.66491620604788e-13</v>
+        <v>-0.01911234194554936</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1765,7 +1765,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4.664970843420106e-13</v>
+        <v>-0.01950403288666215</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1773,7 +1773,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4.664857849195991e-13</v>
+        <v>-0.01871950506953028</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1781,7 +1781,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4.664935485932239e-13</v>
+        <v>-0.01924775647444061</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1789,7 +1789,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>4.664899543598727e-13</v>
+        <v>-0.01899755031140878</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1797,7 +1797,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>4.664977449528496e-13</v>
+        <v>-0.01955312485463102</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1805,7 +1805,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4.664870881012952e-13</v>
+        <v>-0.01880494958775325</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1813,7 +1813,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>4.664911226838319e-13</v>
+        <v>-0.01907782394608838</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1821,7 +1821,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>4.664912051562205e-13</v>
+        <v>-0.01908352856623152</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1829,7 +1829,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>4.664952379793441e-13</v>
+        <v>-0.01936883410390336</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1837,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>4.664966827698115e-13</v>
+        <v>-0.01947436268723461</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1845,7 +1845,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>4.664936782173889e-13</v>
+        <v>-0.0192569636873231</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1853,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-2.402979020608223</v>
+        <v>0.749232955198</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1861,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>4.664776797275013e-13</v>
+        <v>-0.01821358671753741</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1869,7 +1869,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>4.664778747799985e-13</v>
+        <v>-0.01822412098148629</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1877,7 +1877,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>4.664787906864851e-13</v>
+        <v>-0.01827453449563034</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1885,7 +1885,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>4.664951978188981e-13</v>
+        <v>-0.01936592774181042</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1893,7 +1893,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>4.664831680282658e-13</v>
+        <v>-0.01855213112199032</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1901,7 +1901,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>4.664725563875085e-13</v>
+        <v>0.7311432603317456</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1909,7 +1909,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>4.664965852468716e-13</v>
+        <v>-0.01946717913384562</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1917,7 +1917,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>4.664820239584829e-13</v>
+        <v>-0.01848065832907023</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1925,7 +1925,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0.6521510641417722</v>
+        <v>-0.0182637435842448</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1933,7 +1933,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>4.664793377113639e-13</v>
+        <v>-0.01830824388063977</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1941,7 +1941,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>4.664835177370677e-13</v>
+        <v>-0.0185741755748835</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1949,7 +1949,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>0.8974209438083701</v>
+        <v>0.7453451968094781</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1957,7 +1957,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>4.664816604146716e-13</v>
+        <v>-0.01845612601501098</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1965,7 +1965,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>4.664984159146133e-13</v>
+        <v>-0.01960315937657082</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1973,7 +1973,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>4.664828251387408e-13</v>
+        <v>-0.01853060870227724</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1981,7 +1981,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>4.66477549534236e-13</v>
+        <v>-0.01820610837547073</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1989,7 +1989,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>4.664963428705444e-13</v>
+        <v>-0.019449363716421</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1997,7 +1997,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>4.664850696598322e-13</v>
+        <v>-0.01867319810190433</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2005,7 +2005,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>4.664938431125353e-13</v>
+        <v>-0.01926869550644158</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2013,7 +2013,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>4.664796974741326e-13</v>
+        <v>-0.01833106614916399</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2021,7 +2021,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>4.66473385001625e-13</v>
+        <v>0.6957138523236108</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2029,7 +2029,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>4.66497041533346e-13</v>
+        <v>-0.01950086317566575</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2037,7 +2037,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.6551859662729729</v>
+        <v>-0.0182627006791275</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -2045,7 +2045,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>4.664782536187928e-13</v>
+        <v>-0.0182440521426103</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -2053,7 +2053,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>4.665023106014696e-13</v>
+        <v>-0.01989726093012901</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2061,7 +2061,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>4.66497446782363e-13</v>
+        <v>-0.01953092894739928</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2069,7 +2069,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>4.66492747010129e-13</v>
+        <v>-0.01919111216496151</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2077,7 +2077,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>4.664823767133774e-13</v>
+        <v>-0.01850259481728148</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -2085,7 +2085,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>4.664883940246814e-13</v>
+        <v>-0.01889192528663267</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -2093,7 +2093,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>4.664963238735145e-13</v>
+        <v>-0.01944796962336466</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -2101,7 +2101,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>4.664906786516247e-13</v>
+        <v>-0.01904719641869112</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2109,7 +2109,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>4.664795349716061e-13</v>
+        <v>-0.0183207252140634</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2117,7 +2117,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>4.664953206328852e-13</v>
+        <v>-0.01937482014681475</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2125,7 +2125,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>4.664954286490247e-13</v>
+        <v>-0.0193826521483614</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2133,7 +2133,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>4.664898492202537e-13</v>
+        <v>-0.01899037585823373</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -2141,7 +2141,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>4.664932740805163e-13</v>
+        <v>-0.01922830162626882</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2149,7 +2149,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>4.665034649535212e-13</v>
+        <v>-0.8866624473374215</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2157,7 +2157,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>4.66502574091582e-13</v>
+        <v>-0.8354695114681955</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2165,7 +2165,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>4.664899252580043e-13</v>
+        <v>-0.0189955636703553</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2173,7 +2173,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>4.664824118040334e-13</v>
+        <v>-0.01850478170876543</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2181,7 +2181,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>4.664966347126858e-13</v>
+        <v>-0.01947082169376437</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2189,7 +2189,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>4.664769155788786e-13</v>
+        <v>-0.01816393824655939</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2197,7 +2197,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>4.664960122381818e-13</v>
+        <v>-0.01942514872345902</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2205,7 +2205,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>4.664990557512248e-13</v>
+        <v>-0.0196506375910181</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2213,7 +2213,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>4.664845087763694e-13</v>
+        <v>-0.01863718177765158</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2221,7 +2221,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>4.664743022626199e-13</v>
+        <v>0.6369071085536139</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2229,7 +2229,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>4.665027890811998e-13</v>
+        <v>-0.8505462693791914</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2237,7 +2237,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>4.66483879265867e-13</v>
+        <v>-0.01859706754255335</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2245,7 +2245,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>4.664858653017023e-13</v>
+        <v>-0.01872473545891607</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2253,7 +2253,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>4.665029193315406e-13</v>
+        <v>-0.8586402849472062</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2261,7 +2261,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>4.664893618197942e-13</v>
+        <v>-0.01895722421593131</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2269,7 +2269,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>0.897765165562023</v>
+        <v>0.7460799431647391</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2277,7 +2277,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>4.664991411154368e-13</v>
+        <v>-0.01965694505894861</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2285,7 +2285,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>4.6647421827525e-13</v>
+        <v>0.6440332914583019</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2293,7 +2293,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>4.664937085112245e-13</v>
+        <v>-0.01925911737731983</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2301,7 +2301,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>4.664997632619637e-13</v>
+        <v>-0.01970308438866236</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2309,7 +2309,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>4.664939453570221e-13</v>
+        <v>-0.01927598090191606</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2317,7 +2317,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>4.664833978268982e-13</v>
+        <v>-0.01856660598979813</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2325,7 +2325,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>4.664778263878647e-13</v>
+        <v>-0.01822155901239519</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2333,7 +2333,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>4.664992235179287e-13</v>
+        <v>-0.01966303231386526</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2341,7 +2341,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>4.664942976577945e-13</v>
+        <v>-0.01930114901470569</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2349,7 +2349,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>4.664778824276968e-13</v>
+        <v>-0.01822452384534382</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2357,7 +2357,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>4.66494952555297e-13</v>
+        <v>-0.01934820895024297</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2365,7 +2365,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>4.664775897649922e-13</v>
+        <v>-0.01820846835220484</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2373,7 +2373,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>4.66480544800729e-13</v>
+        <v>-0.01838519193320796</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2381,7 +2381,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>4.664929392696508e-13</v>
+        <v>-0.01920465297320734</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2389,7 +2389,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>4.664827486158488e-13</v>
+        <v>-0.01852581770964919</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2397,7 +2397,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>4.664825953434172e-13</v>
+        <v>-0.01851623460914238</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2405,7 +2405,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>4.664838738834028e-13</v>
+        <v>-0.01859672595496505</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2413,7 +2413,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>4.664781621702538e-13</v>
+        <v>-0.01823918137965094</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2421,7 +2421,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>4.664831765904123e-13</v>
+        <v>-0.0185526696901573</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2429,7 +2429,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>0.6918728222059942</v>
+        <v>-0.0182459123068082</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2437,7 +2437,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>4.665010032900744e-13</v>
+        <v>-0.0197991835846949</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2445,7 +2445,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>4.664835493266817e-13</v>
+        <v>-0.01857617166202861</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2453,7 +2453,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>4.664939421674137e-13</v>
+        <v>-0.01927575349041091</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2461,7 +2461,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>4.664817810548281e-13</v>
+        <v>-0.0184637779529077</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2469,7 +2469,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>4.664772677109061e-13</v>
+        <v>-0.01818822217526679</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2477,7 +2477,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>4.664767689048667e-13</v>
+        <v>-0.01815410000929006</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2485,7 +2485,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>4.66493423302658e-13</v>
+        <v>-0.01923886970570107</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2493,7 +2493,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>4.664933754179995e-13</v>
+        <v>-0.01923547659238475</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2501,7 +2501,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>4.664976945184069e-13</v>
+        <v>-0.01954936694224282</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2509,7 +2509,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>4.66497099150198e-13</v>
+        <v>-0.01950512969532689</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2517,7 +2517,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>4.664779290864736e-13</v>
+        <v>-0.01822697295057548</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2525,7 +2525,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>4.66489952637269e-13</v>
+        <v>-0.01899743270654361</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2533,7 +2533,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>4.664894445639116e-13</v>
+        <v>-0.01896283976503164</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2541,7 +2541,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>4.664976135820927e-13</v>
+        <v>-0.01954333911344939</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2549,7 +2549,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>4.664955038178221e-13</v>
+        <v>-0.01938810860182583</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2557,7 +2557,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>4.664880218281473e-13</v>
+        <v>-0.01886700189535631</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2565,7 +2565,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>4.664851698467072e-13</v>
+        <v>-0.01867965885140409</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2573,7 +2573,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>4.664861963414514e-13</v>
+        <v>-0.01874633171292531</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2581,7 +2581,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>4.664860099032132e-13</v>
+        <v>-0.01873415788615973</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2589,7 +2589,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>4.665008494291038e-13</v>
+        <v>-0.01978611739256782</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2597,7 +2597,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>4.664900853108354e-13</v>
+        <v>-0.01900649756260348</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2605,7 +2605,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>4.664929341820764e-13</v>
+        <v>-0.01920429428778572</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2613,7 +2613,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>4.664838043634218e-13</v>
+        <v>-0.0185923160660861</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2621,7 +2621,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>4.664749886178011e-13</v>
+        <v>-0.01805520821671684</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2629,7 +2629,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>4.664730599039279e-13</v>
+        <v>0.7108198960175094</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2637,7 +2637,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>4.664936892801024e-13</v>
+        <v>-0.01925775007426123</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2645,7 +2645,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>4.664920935366179e-13</v>
+        <v>-0.01914529826010878</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2653,7 +2653,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>4.664960021403745e-13</v>
+        <v>-0.01942441075649153</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2661,7 +2661,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>4.664779385436296e-13</v>
+        <v>-0.01822746790417152</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2669,7 +2669,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>4.664826349467569e-13</v>
+        <v>-0.01851870908599945</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2677,7 +2677,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>4.664903057850744e-13</v>
+        <v>-0.01902159010115319</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2685,7 +2685,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>4.664807711082456e-13</v>
+        <v>-0.01839961970396154</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2693,7 +2693,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>4.66479603046089e-13</v>
+        <v>-0.01832505233242615</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2701,7 +2701,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>0.8990003385962474</v>
+        <v>0.748650068375604</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2709,7 +2709,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>4.664950325097478e-13</v>
+        <v>-0.01935397940167341</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2717,7 +2717,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>4.665033981996321e-13</v>
+        <v>-0.8836375962798575</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2725,7 +2725,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>4.664805590989594e-13</v>
+        <v>-0.0183861041567955</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2733,7 +2733,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>4.664880378527037e-13</v>
+        <v>-0.01886807274818287</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2741,7 +2741,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>4.664812313552607e-13</v>
+        <v>-0.01842889406520897</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2749,7 +2749,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>4.664777499038501e-13</v>
+        <v>-0.01821744883217549</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2757,7 +2757,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>4.664847951888972e-13</v>
+        <v>-0.01865554080608967</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2765,7 +2765,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>0.6876670792292234</v>
+        <v>-0.01824821887607458</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2773,7 +2773,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>4.664986567867125e-13</v>
+        <v>-0.01962108022092277</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2781,7 +2781,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>4.664749760326617e-13</v>
+        <v>-0.01805242929218218</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2789,7 +2789,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>4.664888003060197e-13</v>
+        <v>-0.0189192517276501</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2797,7 +2797,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>4.664991270347548e-13</v>
+        <v>-0.01965590484793777</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2805,7 +2805,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>4.664771344442512e-13</v>
+        <v>-0.01817909623487911</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2813,7 +2813,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>4.66503472127245e-13</v>
+        <v>-0.8869819861517966</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2821,7 +2821,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>4.664950141541965e-13</v>
+        <v>-0.01935265417238716</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2829,7 +2829,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>4.66500317394392e-13</v>
+        <v>-0.01974490977024523</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2837,7 +2837,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>4.664816603472564e-13</v>
+        <v>-0.01845612175040253</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2845,7 +2845,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>4.664855131915951e-13</v>
+        <v>-0.01870186326161362</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2853,7 +2853,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>4.664962845021989e-13</v>
+        <v>-0.01944508151057709</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2861,7 +2861,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>4.664983791220332e-13</v>
+        <v>-0.01960041808454315</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2869,7 +2869,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>4.664819480104813e-13</v>
+        <v>-0.01847436684942941</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2877,7 +2877,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>4.665024215598906e-13</v>
+        <v>-0.0199074587960326</v>
       </c>
     </row>
   </sheetData>
@@ -2903,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2911,7 +2911,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2919,7 +2919,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2927,7 +2927,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2935,7 +2935,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2943,7 +2943,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2951,7 +2951,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2959,7 +2959,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2967,7 +2967,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2975,7 +2975,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2983,7 +2983,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2991,7 +2991,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2999,7 +2999,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3007,7 +3007,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3015,7 +3015,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3023,7 +3023,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3031,7 +3031,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3039,7 +3039,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3047,7 +3047,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -3055,7 +3055,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3063,7 +3063,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3071,7 +3071,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -3079,7 +3079,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3087,7 +3087,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3095,7 +3095,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -3103,7 +3103,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -3111,7 +3111,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3119,7 +3119,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -3127,7 +3127,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3135,7 +3135,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -3143,7 +3143,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3151,7 +3151,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3159,7 +3159,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3167,7 +3167,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3175,7 +3175,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3183,7 +3183,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3191,7 +3191,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3199,7 +3199,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -3207,7 +3207,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -3215,7 +3215,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -3223,7 +3223,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -3231,7 +3231,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3239,7 +3239,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -3247,7 +3247,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3255,7 +3255,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3263,7 +3263,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -3271,7 +3271,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3279,7 +3279,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3287,7 +3287,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3295,7 +3295,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -3303,7 +3303,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3311,7 +3311,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3319,7 +3319,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3327,7 +3327,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3335,7 +3335,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -3343,7 +3343,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -3351,7 +3351,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3359,7 +3359,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -3367,7 +3367,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -3375,7 +3375,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -3383,7 +3383,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -3391,7 +3391,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -3399,7 +3399,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -3407,7 +3407,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -3415,7 +3415,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -3423,7 +3423,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -3431,7 +3431,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -3439,7 +3439,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -3447,7 +3447,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -3455,7 +3455,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -3463,7 +3463,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -3471,7 +3471,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -3479,7 +3479,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -3487,7 +3487,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -3495,7 +3495,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -3503,7 +3503,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -3511,7 +3511,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -3519,7 +3519,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -3527,7 +3527,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -3535,7 +3535,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -3543,7 +3543,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -3551,7 +3551,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -3559,7 +3559,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -3567,7 +3567,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -3575,7 +3575,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -3583,7 +3583,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -3591,7 +3591,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -3599,7 +3599,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -3607,7 +3607,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -3615,7 +3615,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -3623,7 +3623,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -3631,7 +3631,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -3639,7 +3639,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -3647,7 +3647,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -3655,7 +3655,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -3663,7 +3663,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -3671,7 +3671,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -3679,7 +3679,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -3687,7 +3687,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -3695,7 +3695,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -3703,7 +3703,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -3711,7 +3711,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -3719,7 +3719,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -3727,7 +3727,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -3735,7 +3735,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -3743,7 +3743,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -3751,7 +3751,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -3759,7 +3759,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -3767,7 +3767,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -3775,7 +3775,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -3783,7 +3783,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -3791,7 +3791,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -3799,7 +3799,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -3807,7 +3807,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -3815,7 +3815,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -3823,7 +3823,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -3831,7 +3831,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -3839,7 +3839,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -3847,7 +3847,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -3855,7 +3855,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -3863,7 +3863,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -3871,7 +3871,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -3879,7 +3879,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -3887,7 +3887,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -3895,7 +3895,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -3903,7 +3903,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -3911,7 +3911,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -3919,7 +3919,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -3927,7 +3927,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -3935,7 +3935,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -3943,7 +3943,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -3951,7 +3951,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -3959,7 +3959,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -3967,7 +3967,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -3975,7 +3975,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -3983,7 +3983,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -3991,7 +3991,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -3999,7 +3999,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -4007,7 +4007,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -4015,7 +4015,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -4023,7 +4023,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -4031,7 +4031,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -4039,7 +4039,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -4047,7 +4047,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -4055,7 +4055,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -4063,7 +4063,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -4071,7 +4071,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -4079,7 +4079,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -4087,7 +4087,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -4095,7 +4095,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The initial variables for the optimization problem have been introduced in the code
</commit_message>
<xml_diff>
--- a/Inverse_Optimization_Related_Problem/temporary_results_inverse_optimization_related_problem/Output.xlsx
+++ b/Inverse_Optimization_Related_Problem/temporary_results_inverse_optimization_related_problem/Output.xlsx
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.07711935043335</v>
+        <v>2.759763717651367</v>
       </c>
     </row>
   </sheetData>
@@ -1685,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-0.01848287542273457</v>
+        <v>-2.167974759139391</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1693,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.6217241268499804</v>
+        <v>-4.45116399200965e-08</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1701,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-0.01862054293010882</v>
+        <v>-4.415042258835782e-08</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1709,7 +1709,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-0.01805540567109086</v>
+        <v>-4.32354106087106e-08</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1717,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-0.01822347440889039</v>
+        <v>8.093617738804096e-08</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1725,7 +1725,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.6894393787108369</v>
+        <v>7.552474221313034e-09</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1733,7 +1733,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-0.01812047942907844</v>
+        <v>-3.280627424941995e-07</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1741,7 +1741,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-0.01841062349237289</v>
+        <v>-2.069951930614636e-08</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1749,7 +1749,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-0.01812674857001915</v>
+        <v>4.864829878640674e-08</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1757,7 +1757,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-0.01911234194554936</v>
+        <v>-4.959913618552829e-08</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1765,7 +1765,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-0.01950403288666215</v>
+        <v>-1.746030840521543e-07</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1773,7 +1773,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-0.01871950506953028</v>
+        <v>-1.833252864424049e-08</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1781,7 +1781,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-0.01924775647444061</v>
+        <v>9.915642948839831e-08</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1789,7 +1789,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-0.01899755031140878</v>
+        <v>2.648559854494112e-08</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1797,7 +1797,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-0.01955312485463102</v>
+        <v>-1.217567644560372e-08</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1805,7 +1805,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>-0.01880494958775325</v>
+        <v>-6.606339109336398e-09</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1813,7 +1813,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-0.01907782394608838</v>
+        <v>6.339272923198112e-08</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1821,7 +1821,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-0.01908352856623152</v>
+        <v>-2.205945713536315e-07</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1829,7 +1829,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>-0.01936883410390336</v>
+        <v>-6.691084765124262e-10</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1837,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>-0.01947436268723461</v>
+        <v>-2.289464003823771e-08</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1845,7 +1845,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>-0.0192569636873231</v>
+        <v>1.240619212193401e-07</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1853,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.749232955198</v>
+        <v>1.033543362961711e-08</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1861,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>-0.01821358671753741</v>
+        <v>-1.713009658489686e-10</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1869,7 +1869,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-0.01822412098148629</v>
+        <v>4.340179400893044e-09</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1877,7 +1877,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>-0.01827453449563034</v>
+        <v>-2.984389887770847e-08</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1885,7 +1885,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>-0.01936592774181042</v>
+        <v>-2.772059944779669e-08</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1893,7 +1893,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>-0.01855213112199032</v>
+        <v>-2.552036657816202e-07</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1901,7 +1901,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.7311432603317456</v>
+        <v>5.810589971611347e-09</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1909,7 +1909,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>-0.01946717913384562</v>
+        <v>3.381507815914042e-08</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1917,7 +1917,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>-0.01848065832907023</v>
+        <v>1.776441693050156e-07</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1925,7 +1925,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>-0.0182637435842448</v>
+        <v>-1.517849802636626e-09</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1933,7 +1933,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>-0.01830824388063977</v>
+        <v>-3.880955507940747e-08</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1941,7 +1941,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>-0.0185741755748835</v>
+        <v>-1.714342229091974e-08</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1949,7 +1949,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>0.7453451968094781</v>
+        <v>-3.336034412824929e-08</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1957,7 +1957,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>-0.01845612601501098</v>
+        <v>-3.519200925135336e-08</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1965,7 +1965,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>-0.01960315937657082</v>
+        <v>-1.652879845655146e-08</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1973,7 +1973,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>-0.01853060870227724</v>
+        <v>-1.143463536867534e-08</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1981,7 +1981,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-0.01820610837547073</v>
+        <v>3.700758963039585e-09</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1989,7 +1989,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>-0.019449363716421</v>
+        <v>5.936741019438803e-09</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1997,7 +1997,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-0.01867319810190433</v>
+        <v>-2.164249976821129e-08</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2005,7 +2005,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>-0.01926869550644158</v>
+        <v>1.63100775687885e-07</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2013,7 +2013,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>-0.01833106614916399</v>
+        <v>5.621459991639807e-12</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2021,7 +2021,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.6957138523236108</v>
+        <v>7.950757664511333e-11</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2029,7 +2029,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>-0.01950086317566575</v>
+        <v>-5.735919433450573e-09</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2037,7 +2037,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>-0.0182627006791275</v>
+        <v>-1.458574304283953e-08</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -2045,7 +2045,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>-0.0182440521426103</v>
+        <v>-1.055091490101525e-07</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -2053,7 +2053,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>-0.01989726093012901</v>
+        <v>-1.697561509188183e-07</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2061,7 +2061,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>-0.01953092894739928</v>
+        <v>4.133592088596386e-08</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2069,7 +2069,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>-0.01919111216496151</v>
+        <v>1.730007636702715e-08</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2077,7 +2077,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>-0.01850259481728148</v>
+        <v>4.068535927044412e-08</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -2085,7 +2085,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>-0.01889192528663267</v>
+        <v>6.537085001944038e-09</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -2093,7 +2093,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>-0.01944796962336466</v>
+        <v>-1.15348482637547e-07</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -2101,7 +2101,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>-0.01904719641869112</v>
+        <v>1.001711075715983e-07</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2109,7 +2109,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>-0.0183207252140634</v>
+        <v>3.709913978792273e-09</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2117,7 +2117,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>-0.01937482014681475</v>
+        <v>-1.176679745659932e-08</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2125,7 +2125,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>-0.0193826521483614</v>
+        <v>2.224995863497323e-08</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2133,7 +2133,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>-0.01899037585823373</v>
+        <v>-1.270585541431134e-07</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -2141,7 +2141,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>-0.01922830162626882</v>
+        <v>8.106246251304943e-08</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2149,7 +2149,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>-0.8866624473374215</v>
+        <v>-5.467600692097412e-09</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2157,7 +2157,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>-0.8354695114681955</v>
+        <v>2.77386120893249e-08</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2165,7 +2165,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>-0.0189955636703553</v>
+        <v>-9.186648532055886e-09</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2173,7 +2173,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>-0.01850478170876543</v>
+        <v>4.037549136183775e-08</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2181,7 +2181,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>-0.01947082169376437</v>
+        <v>-4.630292938992853e-08</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2189,7 +2189,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>-0.01816393824655939</v>
+        <v>1.040243834863739e-07</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2197,7 +2197,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>-0.01942514872345902</v>
+        <v>1.80645184861014e-09</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2205,7 +2205,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>-0.0196506375910181</v>
+        <v>-1.077600528698684e-07</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2213,7 +2213,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>-0.01863718177765158</v>
+        <v>-5.820828488543236e-08</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2221,7 +2221,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>0.6369071085536139</v>
+        <v>-1.808805226306442e-08</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2229,7 +2229,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>-0.8505462693791914</v>
+        <v>1.024334378698204e-08</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2237,7 +2237,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>-0.01859706754255335</v>
+        <v>-2.024487655249814e-07</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2245,7 +2245,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>-0.01872473545891607</v>
+        <v>2.551681388648721e-08</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2253,7 +2253,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>-0.8586402849472062</v>
+        <v>-3.928242378330924e-08</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2261,7 +2261,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>-0.01895722421593131</v>
+        <v>2.272350492237694e-08</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2269,7 +2269,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>0.7460799431647391</v>
+        <v>7.235987430101805e-08</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2277,7 +2277,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>-0.01965694505894861</v>
+        <v>-1.916089047968429e-07</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2285,7 +2285,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>0.6440332914583019</v>
+        <v>1.342259756741415e-09</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2293,7 +2293,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>-0.01925911737731983</v>
+        <v>-9.497211131657001e-08</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2301,7 +2301,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>-0.01970308438866236</v>
+        <v>1.722868296798226e-07</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2309,7 +2309,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>-0.01927598090191606</v>
+        <v>-1.220171065940722e-07</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2317,7 +2317,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>-0.01856660598979813</v>
+        <v>1.97935093018527e-08</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2325,7 +2325,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>-0.01822155901239519</v>
+        <v>9.450571823418436e-08</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2333,7 +2333,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>-0.01966303231386526</v>
+        <v>-7.871571021997854e-10</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2341,7 +2341,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>-0.01930114901470569</v>
+        <v>1.440345818858124e-07</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2349,7 +2349,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>-0.01822452384534382</v>
+        <v>-2.302148006456259</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2357,7 +2357,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>-0.01934820895024297</v>
+        <v>1.092527592872604e-07</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2365,7 +2365,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>-0.01820846835220484</v>
+        <v>5.371973091507048e-08</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2373,7 +2373,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>-0.01838519193320796</v>
+        <v>5.399321283907277e-08</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2381,7 +2381,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>-0.01920465297320734</v>
+        <v>-1.057833161400604e-05</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2389,7 +2389,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>-0.01852581770964919</v>
+        <v>-7.060306122231917e-08</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2397,7 +2397,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>-0.01851623460914238</v>
+        <v>-1.927809880499868e-08</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2405,7 +2405,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>-0.01859672595496505</v>
+        <v>-3.588031859049051e-08</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2413,7 +2413,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>-0.01823918137965094</v>
+        <v>5.096936872694205e-07</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2421,7 +2421,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>-0.0185526696901573</v>
+        <v>9.182938726874839e-09</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2429,7 +2429,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>-0.0182459123068082</v>
+        <v>3.180361619678821e-08</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2437,7 +2437,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>-0.0197991835846949</v>
+        <v>5.487694959434483e-08</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2445,7 +2445,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>-0.01857617166202861</v>
+        <v>2.312016401507387e-09</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2453,7 +2453,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>-0.01927575349041091</v>
+        <v>-1.55395556723788e-08</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2461,7 +2461,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>-0.0184637779529077</v>
+        <v>-2.896988541214729e-08</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2469,7 +2469,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>-0.01818822217526679</v>
+        <v>3.753723692561368e-09</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2477,7 +2477,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>-0.01815410000929006</v>
+        <v>-1.192961469286118e-07</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2485,7 +2485,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>-0.01923886970570107</v>
+        <v>1.554995620528322e-09</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2493,7 +2493,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>-0.01923547659238475</v>
+        <v>-1.394482328826442e-07</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2501,7 +2501,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>-0.01954936694224282</v>
+        <v>4.932626708828706e-08</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2509,7 +2509,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>-0.01950512969532689</v>
+        <v>5.976186072915335e-09</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2517,7 +2517,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>-0.01822697295057548</v>
+        <v>1.598854102732089e-08</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2525,7 +2525,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>-0.01899743270654361</v>
+        <v>6.53008529702027e-09</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2533,7 +2533,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>-0.01896283976503164</v>
+        <v>-1.501150255591833e-09</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2541,7 +2541,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>-0.01954333911344939</v>
+        <v>5.818087132873942e-08</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2549,7 +2549,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>-0.01938810860182583</v>
+        <v>-1.750740436900304e-08</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2557,7 +2557,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>-0.01886700189535631</v>
+        <v>2.278069960869292e-08</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2565,7 +2565,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>-0.01867965885140409</v>
+        <v>-3.907208249400777e-08</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2573,7 +2573,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>-0.01874633171292531</v>
+        <v>8.49082967928591e-08</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2581,7 +2581,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>-0.01873415788615973</v>
+        <v>-2.591590937471511e-08</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2589,7 +2589,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>-0.01978611739256782</v>
+        <v>-4.00330616844083e-08</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2597,7 +2597,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>-0.01900649756260348</v>
+        <v>1.647403877851825e-09</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2605,7 +2605,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>-0.01920429428778572</v>
+        <v>1.375301304799698e-06</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2613,7 +2613,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>-0.0185923160660861</v>
+        <v>-8.916209504041733e-08</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2621,7 +2621,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>-0.01805520821671684</v>
+        <v>-5.601657262944973e-09</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2629,7 +2629,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>0.7108198960175094</v>
+        <v>-2.145201800178086e-06</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2637,7 +2637,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>-0.01925775007426123</v>
+        <v>4.722950850456638e-08</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2645,7 +2645,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>-0.01914529826010878</v>
+        <v>-3.94357428398819e-08</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2653,7 +2653,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>-0.01942441075649153</v>
+        <v>-3.413554619602102e-08</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2661,7 +2661,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>-0.01822746790417152</v>
+        <v>2.904103326016521e-08</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2669,7 +2669,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>-0.01851870908599945</v>
+        <v>-1.525959107995169e-07</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2677,7 +2677,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>-0.01902159010115319</v>
+        <v>2.694446636031043e-08</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2685,7 +2685,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>-0.01839961970396154</v>
+        <v>-6.309130831898615e-10</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2693,7 +2693,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>-0.01832505233242615</v>
+        <v>-2.338792415000123e-07</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2701,7 +2701,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>0.748650068375604</v>
+        <v>1.86536544625206e-08</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2709,7 +2709,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>-0.01935397940167341</v>
+        <v>-1.624981930455002e-08</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2717,7 +2717,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>-0.8836375962798575</v>
+        <v>-9.996524594646756e-09</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2725,7 +2725,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>-0.0183861041567955</v>
+        <v>1.354523578124798e-07</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2733,7 +2733,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>-0.01886807274818287</v>
+        <v>-1.31615459582131e-08</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2741,7 +2741,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>-0.01842889406520897</v>
+        <v>-1.544385619589896e-07</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2749,7 +2749,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>-0.01821744883217549</v>
+        <v>-5.836416983899436e-09</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2757,7 +2757,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>-0.01865554080608967</v>
+        <v>-2.345553402253957e-06</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2765,7 +2765,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>-0.01824821887607458</v>
+        <v>-2.063984807960972e-08</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2773,7 +2773,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>-0.01962108022092277</v>
+        <v>-1.927689995805912e-07</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2781,7 +2781,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>-0.01805242929218218</v>
+        <v>-5.5411686134191e-08</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2789,7 +2789,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>-0.0189192517276501</v>
+        <v>-3.579383455385554e-07</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2797,7 +2797,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>-0.01965590484793777</v>
+        <v>-1.750352539996732e-09</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2805,7 +2805,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>-0.01817909623487911</v>
+        <v>-7.43242433491053e-08</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2813,7 +2813,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>-0.8869819861517966</v>
+        <v>1.221113493756351e-08</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2821,7 +2821,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>-0.01935265417238716</v>
+        <v>4.177898498185276e-08</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2829,7 +2829,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>-0.01974490977024523</v>
+        <v>-3.114706906834342e-08</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2837,7 +2837,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>-0.01845612175040253</v>
+        <v>4.831846846102918e-08</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2845,7 +2845,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>-0.01870186326161362</v>
+        <v>-6.789960101107514e-09</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2853,7 +2853,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>-0.01944508151057709</v>
+        <v>-2.913311648141036e-09</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2861,7 +2861,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>-0.01960041808454315</v>
+        <v>1.810239916731048e-10</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2869,7 +2869,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>-0.01847436684942941</v>
+        <v>-2.291411444444226e-07</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2877,7 +2877,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>-0.0199074587960326</v>
+        <v>3.096566390328359e-09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>